<commit_message>
Berlin70 stability and FOGOffset
</commit_message>
<xml_diff>
--- a/Berlin70/20171211_LS977_FOG_Offset.xlsx
+++ b/Berlin70/20171211_LS977_FOG_Offset.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msu\Desktop\combine all\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chache\Documents\GitHub\DFS\Berlin70\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="0" windowWidth="18000" windowHeight="13560" tabRatio="661"/>
+    <workbookView xWindow="2445" yWindow="0" windowWidth="18000" windowHeight="13560" tabRatio="661" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MicStabEXPOffAGCICFG" sheetId="4" r:id="rId1"/>
@@ -236,19 +236,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -287,7 +287,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -565,16 +571,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +588,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -590,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -598,7 +604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -606,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -614,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -622,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -630,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -638,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -646,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -654,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -662,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -670,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -678,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -686,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -694,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -702,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -710,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -718,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -726,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -734,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -742,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -750,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -758,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -766,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -774,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -782,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -790,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -798,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -806,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -814,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -822,7 +828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -830,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -838,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -846,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -854,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -862,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -870,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -878,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -886,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -894,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -902,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
@@ -910,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -918,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -926,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -934,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
@@ -942,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
@@ -950,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
@@ -958,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -966,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -974,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
@@ -982,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -990,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
@@ -1046,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -1106,12 +1112,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1151,7 +1157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1255,7 +1261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1263,7 +1269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1279,7 +1285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1319,7 +1325,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1335,7 +1341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1359,7 +1365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1383,7 +1389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -1407,7 +1413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -1415,7 +1421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
@@ -1447,7 +1453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -1463,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -1471,7 +1477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -1503,7 +1509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -1535,7 +1541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
@@ -1543,7 +1549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
@@ -1559,7 +1565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -1591,7 +1597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -1641,14 +1647,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1656,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1664,7 +1672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1672,7 +1680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1680,7 +1688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1688,7 +1696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +1704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1704,7 +1712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1712,7 +1720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1720,7 +1728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1728,7 +1736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1752,7 +1760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1760,7 +1768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1768,7 +1776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1776,7 +1784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1784,7 +1792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1800,7 +1808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1808,7 +1816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1816,7 +1824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1824,7 +1832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1832,7 +1840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1840,7 +1848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1856,7 +1864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1864,7 +1872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1872,7 +1880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1880,7 +1888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1888,7 +1896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1896,7 +1904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1904,7 +1912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -1912,7 +1920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -1928,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -1936,7 +1944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -1944,7 +1952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -1952,7 +1960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -1960,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -1968,7 +1976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -1976,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
@@ -1984,7 +1992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -2000,7 +2008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -2008,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
@@ -2016,7 +2024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
@@ -2032,7 +2040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -2040,7 +2048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -2048,7 +2056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
@@ -2056,7 +2064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
@@ -2064,7 +2072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
@@ -2072,7 +2080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
@@ -2080,7 +2088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -2088,7 +2096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
@@ -2096,7 +2104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -2104,7 +2112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
@@ -2112,7 +2120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
@@ -2120,7 +2128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -2128,7 +2136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
@@ -2136,7 +2144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
@@ -2144,7 +2152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
@@ -2152,7 +2160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
@@ -2160,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -2170,6 +2178,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>0</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2180,7 +2194,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>